<commit_message>
new changes in strategy file are added
</commit_message>
<xml_diff>
--- a/My UPSC Strategy.xlsx
+++ b/My UPSC Strategy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hariprasad\Desktop\UPSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D962E61B-3EAF-4EB1-9B3F-295605FF100B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887F031A-6301-4D06-B3B2-0A213DDDE297}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A8AD1D91-E5A0-47C3-9B86-430C59B049E8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
   <si>
     <t>Geography</t>
   </si>
@@ -331,12 +331,77 @@
   <si>
     <t>Start with basic books and keep updating your booklist. Use the following list to select next books</t>
   </si>
+  <si>
+    <t>Exam Dates</t>
+  </si>
+  <si>
+    <t>UPSC CSE 2022 Notification release Date</t>
+  </si>
+  <si>
+    <t>2nd week of February 2022</t>
+  </si>
+  <si>
+    <t>Date of Application form availability</t>
+  </si>
+  <si>
+    <t>Online Application form Last date Submit</t>
+  </si>
+  <si>
+    <t>Prelims Exam Admit Card</t>
+  </si>
+  <si>
+    <t>Exam date (Prelims)</t>
+  </si>
+  <si>
+    <t>Preliminary exam result</t>
+  </si>
+  <si>
+    <t>Admit Card for Main Exam</t>
+  </si>
+  <si>
+    <t>September 2022  </t>
+  </si>
+  <si>
+    <t>Exam Date (Main)</t>
+  </si>
+  <si>
+    <t>September 2022 </t>
+  </si>
+  <si>
+    <t>Final result Announced</t>
+  </si>
+  <si>
+    <r>
+      <t>January </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>2023</t>
+    </r>
+  </si>
+  <si>
+    <t>Events </t>
+  </si>
+  <si>
+    <t>March 22 to June 22</t>
+  </si>
+  <si>
+    <t>Current Status</t>
+  </si>
+  <si>
+    <t>Try to finish polity and economics first so that you will understand current affairs. Start with basic books. Atleast finish NCERTs before you completely sit on UPSC preparation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,16 +415,54 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -396,26 +499,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -423,8 +559,8 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="medium">
@@ -433,13 +569,11 @@
         <bottom style="medium">
           <color rgb="FFA3A3A3"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="medium">
@@ -448,13 +582,11 @@
         <bottom style="medium">
           <color rgb="FFA3A3A3"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="medium">
@@ -463,13 +595,11 @@
         <bottom style="medium">
           <color rgb="FFA3A3A3"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="medium">
@@ -478,13 +608,11 @@
         <bottom style="medium">
           <color rgb="FFA3A3A3"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="medium">
@@ -493,13 +621,11 @@
         <bottom style="medium">
           <color rgb="FFA3A3A3"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top style="medium">
@@ -508,8 +634,6 @@
         <bottom style="medium">
           <color rgb="FFA3A3A3"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -536,7 +660,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -546,7 +670,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -562,8 +686,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3FF3E4BA-FF09-4DFB-8987-F2913B196AFE}" name="Table1" displayName="Table1" ref="C6:H25" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="C6:H25" xr:uid="{823D61BB-7A9C-4231-BC18-FB153482B20E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3FF3E4BA-FF09-4DFB-8987-F2913B196AFE}" name="Table1" displayName="Table1" ref="C15:H34" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="C15:H34" xr:uid="{823D61BB-7A9C-4231-BC18-FB153482B20E}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D5AA82E9-6C4A-47DE-9721-688747BA4601}" name="Topic" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{67FA8CA1-5C38-418C-8703-147050082443}" name="Akshat Jain Books" dataDxfId="4"/>
@@ -873,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E02B99-EFA9-4A7F-B955-F322558B5581}">
-  <dimension ref="C4:H25"/>
+  <dimension ref="C2:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -889,322 +1013,483 @@
     <col min="8" max="8" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+    <row r="2" spans="3:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="C2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="6" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="3" t="s">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="C4" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="9">
+        <v>44593</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="3:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="C5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="9">
+        <v>44621</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="9">
+        <v>44713</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="3:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="C7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="9">
+        <v>44713</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="3:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="C8" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="9">
+        <v>44774</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="3:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="C9" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="3:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="C10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="3:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="C11" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H15" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="3:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="2" t="s">
+    <row r="16" spans="3:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="3:8" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="2" t="s">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="3:8" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="3:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="2" t="s">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="3:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="3:8" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="2" t="s">
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="3:8" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="3:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="2" t="s">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="3:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="3:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="2" t="s">
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="3:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="3:8" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="2" t="s">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="3:8" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="3:8" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="3:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="3:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="3:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="3:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="3:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="3:8" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="3:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="3:8" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="3:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="3:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="3:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="3:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="3:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="3:8" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="3:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="3:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="2" t="s">
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="3:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2" t="s">
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="3:8" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="4" t="s">
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="3:8" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D33" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4" t="s">
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="3:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="C25" s="4" t="s">
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C34" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D34" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4" t="s">
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="H25" s="4"/>
+      <c r="H34" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>